<commit_message>
:white_check_mark: 2nd test passed.
</commit_message>
<xml_diff>
--- a/examples/save_result_example.xlsx
+++ b/examples/save_result_example.xlsx
@@ -454,7 +454,7 @@
         <v>120</v>
       </c>
       <c r="C2" t="n">
-        <v>54.16666666666666</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="3">
@@ -465,7 +465,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>63.33333333333333</v>
+        <v>56.66666666666666</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +487,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="n">
-        <v>66.66666666666666</v>
+        <v>56.66666666666666</v>
       </c>
     </row>
     <row r="6">
@@ -531,7 +531,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="n">
-        <v>93.33333333333333</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">

</xml_diff>